<commit_message>
Fix add equipo  and Project Creation
</commit_message>
<xml_diff>
--- a/ExcelFiles/ProductosM.xlsx
+++ b/ExcelFiles/ProductosM.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CoteL\Desktop\Intech\Excel cargas masivas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Intec\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB6287C-0496-44AD-BFED-295A1522C514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6773ACE-157C-4900-8E9A-507CBCB0CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$168</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,28 +27,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Sub categoria</t>
+  </si>
+  <si>
+    <t>Nombre producto</t>
+  </si>
+  <si>
     <t>marca</t>
   </si>
   <si>
     <t>modelo</t>
   </si>
   <si>
-    <t>categoria asociada</t>
-  </si>
-  <si>
-    <t>item asociado</t>
+    <t>cantidad</t>
   </si>
   <si>
     <t>precio compra</t>
   </si>
   <si>
     <t>precio estimado arriendo</t>
-  </si>
-  <si>
-    <t>Nombre producto</t>
-  </si>
-  <si>
-    <t>cantidad</t>
   </si>
 </sst>
 </file>
@@ -68,7 +65,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,7 +81,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,8 +115,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,340 +399,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H168" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>